<commit_message>
intente leer el qmd y salio mal :c
</commit_message>
<xml_diff>
--- a/hitters.xlsx
+++ b/hitters.xlsx
@@ -533,7 +533,7 @@
         <v>10</v>
       </c>
       <c r="S2" t="n">
-        <v>475</v>
+        <v>6.16331480403464</v>
       </c>
       <c r="T2" t="s">
         <v>20</v>
@@ -595,7 +595,7 @@
         <v>14</v>
       </c>
       <c r="S3" t="n">
-        <v>480</v>
+        <v>6.17378610390194</v>
       </c>
       <c r="T3" t="s">
         <v>22</v>
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="S4" t="n">
-        <v>500</v>
+        <v>6.21460809842219</v>
       </c>
       <c r="T4" t="s">
         <v>20</v>
@@ -719,7 +719,7 @@
         <v>4</v>
       </c>
       <c r="S5" t="n">
-        <v>91.5</v>
+        <v>4.51633897228148</v>
       </c>
       <c r="T5" t="s">
         <v>20</v>
@@ -781,7 +781,7 @@
         <v>25</v>
       </c>
       <c r="S6" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T6" t="s">
         <v>22</v>
@@ -843,7 +843,7 @@
         <v>7</v>
       </c>
       <c r="S7" t="n">
-        <v>70</v>
+        <v>4.24849524204936</v>
       </c>
       <c r="T7" t="s">
         <v>22</v>
@@ -905,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="S8" t="n">
-        <v>100</v>
+        <v>4.60517018598809</v>
       </c>
       <c r="T8" t="s">
         <v>22</v>
@@ -967,7 +967,7 @@
         <v>19</v>
       </c>
       <c r="S9" t="n">
-        <v>75</v>
+        <v>4.31748811353631</v>
       </c>
       <c r="T9" t="s">
         <v>20</v>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>1100</v>
+        <v>7.00306545878646</v>
       </c>
       <c r="T10" t="s">
         <v>22</v>
@@ -1091,7 +1091,7 @@
         <v>22</v>
       </c>
       <c r="S11" t="n">
-        <v>517.143</v>
+        <v>6.24831943200756</v>
       </c>
       <c r="T11" t="s">
         <v>22</v>
@@ -1153,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="S12" t="n">
-        <v>512.5</v>
+        <v>6.23930071101256</v>
       </c>
       <c r="T12" t="s">
         <v>20</v>
@@ -1215,7 +1215,7 @@
         <v>7</v>
       </c>
       <c r="S13" t="n">
-        <v>550</v>
+        <v>6.30991827822652</v>
       </c>
       <c r="T13" t="s">
         <v>20</v>
@@ -1277,7 +1277,7 @@
         <v>6</v>
       </c>
       <c r="S14" t="n">
-        <v>700</v>
+        <v>6.5510803350434</v>
       </c>
       <c r="T14" t="s">
         <v>22</v>
@@ -1339,7 +1339,7 @@
         <v>8</v>
       </c>
       <c r="S15" t="n">
-        <v>240</v>
+        <v>5.48063892334199</v>
       </c>
       <c r="T15" t="s">
         <v>20</v>
@@ -1401,7 +1401,7 @@
         <v>10</v>
       </c>
       <c r="S16" t="n">
-        <v>775</v>
+        <v>6.65286302935335</v>
       </c>
       <c r="T16" t="s">
         <v>20</v>
@@ -1463,7 +1463,7 @@
         <v>16</v>
       </c>
       <c r="S17" t="n">
-        <v>175</v>
+        <v>5.16478597392351</v>
       </c>
       <c r="T17" t="s">
         <v>22</v>
@@ -1525,7 +1525,7 @@
         <v>2</v>
       </c>
       <c r="S18" t="n">
-        <v>135</v>
+        <v>4.90527477843843</v>
       </c>
       <c r="T18" t="s">
         <v>20</v>
@@ -1587,7 +1587,7 @@
         <v>5</v>
       </c>
       <c r="S19" t="n">
-        <v>100</v>
+        <v>4.60517018598809</v>
       </c>
       <c r="T19" t="s">
         <v>20</v>
@@ -1649,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="S20" t="n">
-        <v>115</v>
+        <v>4.74493212836325</v>
       </c>
       <c r="T20" t="s">
         <v>20</v>
@@ -1711,7 +1711,7 @@
         <v>3</v>
       </c>
       <c r="S21" t="n">
-        <v>600</v>
+        <v>6.39692965521615</v>
       </c>
       <c r="T21" t="s">
         <v>20</v>
@@ -1773,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="S22" t="n">
-        <v>776.667</v>
+        <v>6.65501168707609</v>
       </c>
       <c r="T22" t="s">
         <v>22</v>
@@ -1835,7 +1835,7 @@
         <v>3</v>
       </c>
       <c r="S23" t="n">
-        <v>765</v>
+        <v>6.63987583382654</v>
       </c>
       <c r="T23" t="s">
         <v>22</v>
@@ -1897,7 +1897,7 @@
         <v>3</v>
       </c>
       <c r="S24" t="n">
-        <v>708.333</v>
+        <v>6.56291432210206</v>
       </c>
       <c r="T24" t="s">
         <v>20</v>
@@ -1959,7 +1959,7 @@
         <v>13</v>
       </c>
       <c r="S25" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T25" t="s">
         <v>20</v>
@@ -2021,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="S26" t="n">
-        <v>625</v>
+        <v>6.4377516497364</v>
       </c>
       <c r="T26" t="s">
         <v>20</v>
@@ -2083,7 +2083,7 @@
         <v>3</v>
       </c>
       <c r="S27" t="n">
-        <v>900</v>
+        <v>6.80239476332431</v>
       </c>
       <c r="T27" t="s">
         <v>22</v>
@@ -2145,7 +2145,7 @@
         <v>4</v>
       </c>
       <c r="S28" t="n">
-        <v>110</v>
+        <v>4.70048036579242</v>
       </c>
       <c r="T28" t="s">
         <v>20</v>
@@ -2207,7 +2207,7 @@
         <v>25</v>
       </c>
       <c r="S29" t="n">
-        <v>612.5</v>
+        <v>6.41754894241888</v>
       </c>
       <c r="T29" t="s">
         <v>22</v>
@@ -2269,7 +2269,7 @@
         <v>5</v>
       </c>
       <c r="S30" t="n">
-        <v>300</v>
+        <v>5.7037824746562</v>
       </c>
       <c r="T30" t="s">
         <v>22</v>
@@ -2331,7 +2331,7 @@
         <v>24</v>
       </c>
       <c r="S31" t="n">
-        <v>850</v>
+        <v>6.74523634948436</v>
       </c>
       <c r="T31" t="s">
         <v>20</v>
@@ -2393,7 +2393,7 @@
         <v>6</v>
       </c>
       <c r="S32" t="n">
-        <v>90</v>
+        <v>4.49980967033027</v>
       </c>
       <c r="T32" t="s">
         <v>20</v>
@@ -2455,7 +2455,7 @@
         <v>5</v>
       </c>
       <c r="S33" t="n">
-        <v>67.5</v>
+        <v>4.21212759787848</v>
       </c>
       <c r="T33" t="s">
         <v>22</v>
@@ -2517,7 +2517,7 @@
         <v>1</v>
       </c>
       <c r="S34" t="n">
-        <v>180</v>
+        <v>5.19295685089021</v>
       </c>
       <c r="T34" t="s">
         <v>22</v>
@@ -2579,7 +2579,7 @@
         <v>4</v>
       </c>
       <c r="S35" t="n">
-        <v>305</v>
+        <v>5.72031177660741</v>
       </c>
       <c r="T35" t="s">
         <v>22</v>
@@ -2641,7 +2641,7 @@
         <v>18</v>
       </c>
       <c r="S36" t="n">
-        <v>215</v>
+        <v>5.37063802812766</v>
       </c>
       <c r="T36" t="s">
         <v>20</v>
@@ -2703,7 +2703,7 @@
         <v>4</v>
       </c>
       <c r="S37" t="n">
-        <v>247.5</v>
+        <v>5.51141058200874</v>
       </c>
       <c r="T37" t="s">
         <v>22</v>
@@ -2765,7 +2765,7 @@
         <v>9</v>
       </c>
       <c r="S38" t="n">
-        <v>815</v>
+        <v>6.70318811324086</v>
       </c>
       <c r="T38" t="s">
         <v>20</v>
@@ -2827,7 +2827,7 @@
         <v>4</v>
       </c>
       <c r="S39" t="n">
-        <v>875</v>
+        <v>6.77422388635761</v>
       </c>
       <c r="T39" t="s">
         <v>22</v>
@@ -2889,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="S40" t="n">
-        <v>70</v>
+        <v>4.24849524204936</v>
       </c>
       <c r="T40" t="s">
         <v>20</v>
@@ -2951,7 +2951,7 @@
         <v>4</v>
       </c>
       <c r="S41" t="n">
-        <v>1200</v>
+        <v>7.09007683577609</v>
       </c>
       <c r="T41" t="s">
         <v>22</v>
@@ -3013,7 +3013,7 @@
         <v>5</v>
       </c>
       <c r="S42" t="n">
-        <v>675</v>
+        <v>6.51471269087253</v>
       </c>
       <c r="T42" t="s">
         <v>22</v>
@@ -3075,7 +3075,7 @@
         <v>3</v>
       </c>
       <c r="S43" t="n">
-        <v>415</v>
+        <v>6.0282785202307</v>
       </c>
       <c r="T43" t="s">
         <v>20</v>
@@ -3137,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="S44" t="n">
-        <v>340</v>
+        <v>5.82894561761021</v>
       </c>
       <c r="T44" t="s">
         <v>20</v>
@@ -3199,7 +3199,7 @@
         <v>7</v>
       </c>
       <c r="S45" t="n">
-        <v>416.667</v>
+        <v>6.03228734162792</v>
       </c>
       <c r="T45" t="s">
         <v>20</v>
@@ -3261,7 +3261,7 @@
         <v>13</v>
       </c>
       <c r="S46" t="n">
-        <v>1350</v>
+        <v>7.20785987143248</v>
       </c>
       <c r="T46" t="s">
         <v>22</v>
@@ -3323,7 +3323,7 @@
         <v>10</v>
       </c>
       <c r="S47" t="n">
-        <v>90</v>
+        <v>4.49980967033027</v>
       </c>
       <c r="T47" t="s">
         <v>22</v>
@@ -3385,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="S48" t="n">
-        <v>275</v>
+        <v>5.61677109766657</v>
       </c>
       <c r="T48" t="s">
         <v>20</v>
@@ -3447,7 +3447,7 @@
         <v>13</v>
       </c>
       <c r="S49" t="n">
-        <v>230</v>
+        <v>5.4380793089232</v>
       </c>
       <c r="T49" t="s">
         <v>22</v>
@@ -3509,7 +3509,7 @@
         <v>11</v>
       </c>
       <c r="S50" t="n">
-        <v>225</v>
+        <v>5.41610040220442</v>
       </c>
       <c r="T50" t="s">
         <v>20</v>
@@ -3571,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="S51" t="n">
-        <v>950</v>
+        <v>6.85646198459459</v>
       </c>
       <c r="T51" t="s">
         <v>22</v>
@@ -3633,7 +3633,7 @@
         <v>5</v>
       </c>
       <c r="S52" t="n">
-        <v>75</v>
+        <v>4.31748811353631</v>
       </c>
       <c r="T52" t="s">
         <v>22</v>
@@ -3695,7 +3695,7 @@
         <v>23</v>
       </c>
       <c r="S53" t="n">
-        <v>105</v>
+        <v>4.65396035015752</v>
       </c>
       <c r="T53" t="s">
         <v>22</v>
@@ -3757,7 +3757,7 @@
         <v>10</v>
       </c>
       <c r="S54" t="n">
-        <v>320</v>
+        <v>5.76832099579377</v>
       </c>
       <c r="T54" t="s">
         <v>20</v>
@@ -3819,7 +3819,7 @@
         <v>12</v>
       </c>
       <c r="S55" t="n">
-        <v>850</v>
+        <v>6.74523634948436</v>
       </c>
       <c r="T55" t="s">
         <v>22</v>
@@ -3881,7 +3881,7 @@
         <v>2</v>
       </c>
       <c r="S56" t="n">
-        <v>535</v>
+        <v>6.28226674689601</v>
       </c>
       <c r="T56" t="s">
         <v>22</v>
@@ -3943,7 +3943,7 @@
         <v>5</v>
       </c>
       <c r="S57" t="n">
-        <v>933.333</v>
+        <v>6.83876205035226</v>
       </c>
       <c r="T57" t="s">
         <v>22</v>
@@ -4005,7 +4005,7 @@
         <v>8</v>
       </c>
       <c r="S58" t="n">
-        <v>850</v>
+        <v>6.74523634948436</v>
       </c>
       <c r="T58" t="s">
         <v>20</v>
@@ -4067,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="S59" t="n">
-        <v>210</v>
+        <v>5.34710753071747</v>
       </c>
       <c r="T59" t="s">
         <v>22</v>
@@ -4129,7 +4129,7 @@
         <v>4</v>
       </c>
       <c r="S60" t="n">
-        <v>325</v>
+        <v>5.78382518232974</v>
       </c>
       <c r="T60" t="s">
         <v>22</v>
@@ -4191,7 +4191,7 @@
         <v>9</v>
       </c>
       <c r="S61" t="n">
-        <v>275</v>
+        <v>5.61677109766657</v>
       </c>
       <c r="T61" t="s">
         <v>22</v>
@@ -4253,7 +4253,7 @@
         <v>8</v>
       </c>
       <c r="S62" t="n">
-        <v>450</v>
+        <v>6.10924758276437</v>
       </c>
       <c r="T62" t="s">
         <v>20</v>
@@ -4315,7 +4315,7 @@
         <v>6</v>
       </c>
       <c r="S63" t="n">
-        <v>1975</v>
+        <v>7.58832367733522</v>
       </c>
       <c r="T63" t="s">
         <v>22</v>
@@ -4377,7 +4377,7 @@
         <v>6</v>
       </c>
       <c r="S64" t="n">
-        <v>1900</v>
+        <v>7.54960916515453</v>
       </c>
       <c r="T64" t="s">
         <v>20</v>
@@ -4439,7 +4439,7 @@
         <v>2</v>
       </c>
       <c r="S65" t="n">
-        <v>600</v>
+        <v>6.39692965521615</v>
       </c>
       <c r="T65" t="s">
         <v>22</v>
@@ -4501,7 +4501,7 @@
         <v>9</v>
       </c>
       <c r="S66" t="n">
-        <v>1041.667</v>
+        <v>6.94857759350234</v>
       </c>
       <c r="T66" t="s">
         <v>20</v>
@@ -4563,7 +4563,7 @@
         <v>2</v>
       </c>
       <c r="S67" t="n">
-        <v>110</v>
+        <v>4.70048036579242</v>
       </c>
       <c r="T67" t="s">
         <v>22</v>
@@ -4625,7 +4625,7 @@
         <v>1</v>
       </c>
       <c r="S68" t="n">
-        <v>260</v>
+        <v>5.56068163101553</v>
       </c>
       <c r="T68" t="s">
         <v>22</v>
@@ -4687,7 +4687,7 @@
         <v>18</v>
       </c>
       <c r="S69" t="n">
-        <v>475</v>
+        <v>6.16331480403464</v>
       </c>
       <c r="T69" t="s">
         <v>22</v>
@@ -4749,7 +4749,7 @@
         <v>4</v>
       </c>
       <c r="S70" t="n">
-        <v>431.5</v>
+        <v>6.06726751052348</v>
       </c>
       <c r="T70" t="s">
         <v>22</v>
@@ -4811,7 +4811,7 @@
         <v>6</v>
       </c>
       <c r="S71" t="n">
-        <v>1220</v>
+        <v>7.1066061377273</v>
       </c>
       <c r="T71" t="s">
         <v>20</v>
@@ -4873,7 +4873,7 @@
         <v>26</v>
       </c>
       <c r="S72" t="n">
-        <v>70</v>
+        <v>4.24849524204936</v>
       </c>
       <c r="T72" t="s">
         <v>22</v>
@@ -4935,7 +4935,7 @@
         <v>8</v>
       </c>
       <c r="S73" t="n">
-        <v>145</v>
+        <v>4.97673374242057</v>
       </c>
       <c r="T73" t="s">
         <v>22</v>
@@ -4997,7 +4997,7 @@
         <v>9</v>
       </c>
       <c r="S74" t="n">
-        <v>595</v>
+        <v>6.38856140554563</v>
       </c>
       <c r="T74" t="s">
         <v>20</v>
@@ -5059,7 +5059,7 @@
         <v>5</v>
       </c>
       <c r="S75" t="n">
-        <v>1861.46</v>
+        <v>7.52911640503463</v>
       </c>
       <c r="T75" t="s">
         <v>22</v>
@@ -5121,7 +5121,7 @@
         <v>7</v>
       </c>
       <c r="S76" t="n">
-        <v>300</v>
+        <v>5.7037824746562</v>
       </c>
       <c r="T76" t="s">
         <v>20</v>
@@ -5183,7 +5183,7 @@
         <v>3</v>
       </c>
       <c r="S77" t="n">
-        <v>490</v>
+        <v>6.19440539110467</v>
       </c>
       <c r="T77" t="s">
         <v>20</v>
@@ -5245,7 +5245,7 @@
         <v>13</v>
       </c>
       <c r="S78" t="n">
-        <v>2460</v>
+        <v>7.80791662892641</v>
       </c>
       <c r="T78" t="s">
         <v>22</v>
@@ -5307,7 +5307,7 @@
         <v>10</v>
       </c>
       <c r="S79" t="n">
-        <v>375</v>
+        <v>5.92692602597041</v>
       </c>
       <c r="T79" t="s">
         <v>22</v>
@@ -5369,7 +5369,7 @@
         <v>10</v>
       </c>
       <c r="S80" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T80" t="s">
         <v>22</v>
@@ -5431,7 +5431,7 @@
         <v>10</v>
       </c>
       <c r="S81" t="n">
-        <v>1175</v>
+        <v>7.06902342657826</v>
       </c>
       <c r="T81" t="s">
         <v>22</v>
@@ -5493,7 +5493,7 @@
         <v>12</v>
       </c>
       <c r="S82" t="n">
-        <v>70</v>
+        <v>4.24849524204936</v>
       </c>
       <c r="T82" t="s">
         <v>22</v>
@@ -5555,7 +5555,7 @@
         <v>16</v>
       </c>
       <c r="S83" t="n">
-        <v>1500</v>
+        <v>7.3132203870903</v>
       </c>
       <c r="T83" t="s">
         <v>22</v>
@@ -5617,7 +5617,7 @@
         <v>3</v>
       </c>
       <c r="S84" t="n">
-        <v>385</v>
+        <v>5.95324333428778</v>
       </c>
       <c r="T84" t="s">
         <v>22</v>
@@ -5679,7 +5679,7 @@
         <v>8</v>
       </c>
       <c r="S85" t="n">
-        <v>1925.571</v>
+        <v>7.56297782611449</v>
       </c>
       <c r="T85" t="s">
         <v>20</v>
@@ -5741,7 +5741,7 @@
         <v>11</v>
       </c>
       <c r="S86" t="n">
-        <v>215</v>
+        <v>5.37063802812766</v>
       </c>
       <c r="T86" t="s">
         <v>20</v>
@@ -5803,7 +5803,7 @@
         <v>21</v>
       </c>
       <c r="S87" t="n">
-        <v>900</v>
+        <v>6.80239476332431</v>
       </c>
       <c r="T87" t="s">
         <v>22</v>
@@ -5865,7 +5865,7 @@
         <v>26</v>
       </c>
       <c r="S88" t="n">
-        <v>155</v>
+        <v>5.04342511691925</v>
       </c>
       <c r="T88" t="s">
         <v>22</v>
@@ -5927,7 +5927,7 @@
         <v>5</v>
       </c>
       <c r="S89" t="n">
-        <v>700</v>
+        <v>6.5510803350434</v>
       </c>
       <c r="T89" t="s">
         <v>22</v>
@@ -5989,7 +5989,7 @@
         <v>19</v>
       </c>
       <c r="S90" t="n">
-        <v>535</v>
+        <v>6.28226674689601</v>
       </c>
       <c r="T90" t="s">
         <v>20</v>
@@ -6051,7 +6051,7 @@
         <v>12</v>
       </c>
       <c r="S91" t="n">
-        <v>362.5</v>
+        <v>5.89302447429473</v>
       </c>
       <c r="T91" t="s">
         <v>22</v>
@@ -6113,7 +6113,7 @@
         <v>9</v>
       </c>
       <c r="S92" t="n">
-        <v>733.333</v>
+        <v>6.59759989613274</v>
       </c>
       <c r="T92" t="s">
         <v>20</v>
@@ -6175,7 +6175,7 @@
         <v>16</v>
       </c>
       <c r="S93" t="n">
-        <v>200</v>
+        <v>5.29831736654804</v>
       </c>
       <c r="T93" t="s">
         <v>20</v>
@@ -6237,7 +6237,7 @@
         <v>7</v>
       </c>
       <c r="S94" t="n">
-        <v>400</v>
+        <v>5.99146454710798</v>
       </c>
       <c r="T94" t="s">
         <v>22</v>
@@ -6299,7 +6299,7 @@
         <v>4</v>
       </c>
       <c r="S95" t="n">
-        <v>400</v>
+        <v>5.99146454710798</v>
       </c>
       <c r="T95" t="s">
         <v>22</v>
@@ -6361,7 +6361,7 @@
         <v>20</v>
       </c>
       <c r="S96" t="n">
-        <v>737.5</v>
+        <v>6.60326608821398</v>
       </c>
       <c r="T96" t="s">
         <v>20</v>
@@ -6423,7 +6423,7 @@
         <v>5</v>
       </c>
       <c r="S97" t="n">
-        <v>500</v>
+        <v>6.21460809842219</v>
       </c>
       <c r="T97" t="s">
         <v>22</v>
@@ -6485,7 +6485,7 @@
         <v>1</v>
       </c>
       <c r="S98" t="n">
-        <v>600</v>
+        <v>6.39692965521615</v>
       </c>
       <c r="T98" t="s">
         <v>22</v>
@@ -6547,7 +6547,7 @@
         <v>4</v>
       </c>
       <c r="S99" t="n">
-        <v>662.5</v>
+        <v>6.49602055786038</v>
       </c>
       <c r="T99" t="s">
         <v>20</v>
@@ -6609,7 +6609,7 @@
         <v>5</v>
       </c>
       <c r="S100" t="n">
-        <v>950</v>
+        <v>6.85646198459459</v>
       </c>
       <c r="T100" t="s">
         <v>22</v>
@@ -6671,7 +6671,7 @@
         <v>15</v>
       </c>
       <c r="S101" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T101" t="s">
         <v>20</v>
@@ -6733,7 +6733,7 @@
         <v>20</v>
       </c>
       <c r="S102" t="n">
-        <v>297.5</v>
+        <v>5.69541422498568</v>
       </c>
       <c r="T102" t="s">
         <v>20</v>
@@ -6795,7 +6795,7 @@
         <v>0</v>
       </c>
       <c r="S103" t="n">
-        <v>325</v>
+        <v>5.78382518232974</v>
       </c>
       <c r="T103" t="s">
         <v>22</v>
@@ -6857,7 +6857,7 @@
         <v>16</v>
       </c>
       <c r="S104" t="n">
-        <v>87.5</v>
+        <v>4.47163879336357</v>
       </c>
       <c r="T104" t="s">
         <v>22</v>
@@ -6919,7 +6919,7 @@
         <v>1</v>
       </c>
       <c r="S105" t="n">
-        <v>175</v>
+        <v>5.16478597392351</v>
       </c>
       <c r="T105" t="s">
         <v>20</v>
@@ -6981,7 +6981,7 @@
         <v>2</v>
       </c>
       <c r="S106" t="n">
-        <v>90</v>
+        <v>4.49980967033027</v>
       </c>
       <c r="T106" t="s">
         <v>20</v>
@@ -7043,7 +7043,7 @@
         <v>3</v>
       </c>
       <c r="S107" t="n">
-        <v>1237.5</v>
+        <v>7.12084849444285</v>
       </c>
       <c r="T107" t="s">
         <v>22</v>
@@ -7105,7 +7105,7 @@
         <v>13</v>
       </c>
       <c r="S108" t="n">
-        <v>430</v>
+        <v>6.06378520868761</v>
       </c>
       <c r="T108" t="s">
         <v>22</v>
@@ -7167,7 +7167,7 @@
         <v>9</v>
       </c>
       <c r="S109" t="n">
-        <v>100</v>
+        <v>4.60517018598809</v>
       </c>
       <c r="T109" t="s">
         <v>20</v>
@@ -7229,7 +7229,7 @@
         <v>14</v>
       </c>
       <c r="S110" t="n">
-        <v>165</v>
+        <v>5.10594547390058</v>
       </c>
       <c r="T110" t="s">
         <v>22</v>
@@ -7291,7 +7291,7 @@
         <v>6</v>
       </c>
       <c r="S111" t="n">
-        <v>250</v>
+        <v>5.52146091786225</v>
       </c>
       <c r="T111" t="s">
         <v>22</v>
@@ -7353,7 +7353,7 @@
         <v>3</v>
       </c>
       <c r="S112" t="n">
-        <v>1300</v>
+        <v>7.17011954344963</v>
       </c>
       <c r="T112" t="s">
         <v>20</v>
@@ -7415,7 +7415,7 @@
         <v>4</v>
       </c>
       <c r="S113" t="n">
-        <v>773.333</v>
+        <v>6.65070974495767</v>
       </c>
       <c r="T113" t="s">
         <v>20</v>
@@ -7477,7 +7477,7 @@
         <v>8</v>
       </c>
       <c r="S114" t="n">
-        <v>1008.333</v>
+        <v>6.91605375121827</v>
       </c>
       <c r="T114" t="s">
         <v>20</v>
@@ -7539,7 +7539,7 @@
         <v>0</v>
       </c>
       <c r="S115" t="n">
-        <v>275</v>
+        <v>5.61677109766657</v>
       </c>
       <c r="T115" t="s">
         <v>22</v>
@@ -7601,7 +7601,7 @@
         <v>18</v>
       </c>
       <c r="S116" t="n">
-        <v>775</v>
+        <v>6.65286302935335</v>
       </c>
       <c r="T116" t="s">
         <v>22</v>
@@ -7663,7 +7663,7 @@
         <v>10</v>
       </c>
       <c r="S117" t="n">
-        <v>850</v>
+        <v>6.74523634948436</v>
       </c>
       <c r="T117" t="s">
         <v>22</v>
@@ -7725,7 +7725,7 @@
         <v>0</v>
       </c>
       <c r="S118" t="n">
-        <v>365</v>
+        <v>5.89989735358249</v>
       </c>
       <c r="T118" t="s">
         <v>22</v>
@@ -7787,7 +7787,7 @@
         <v>2</v>
       </c>
       <c r="S119" t="n">
-        <v>95</v>
+        <v>4.55387689160054</v>
       </c>
       <c r="T119" t="s">
         <v>22</v>
@@ -7849,7 +7849,7 @@
         <v>2</v>
       </c>
       <c r="S120" t="n">
-        <v>110</v>
+        <v>4.70048036579242</v>
       </c>
       <c r="T120" t="s">
         <v>20</v>
@@ -7911,7 +7911,7 @@
         <v>5</v>
       </c>
       <c r="S121" t="n">
-        <v>100</v>
+        <v>4.60517018598809</v>
       </c>
       <c r="T121" t="s">
         <v>20</v>
@@ -7973,7 +7973,7 @@
         <v>20</v>
       </c>
       <c r="S122" t="n">
-        <v>277.5</v>
+        <v>5.62582093318649</v>
       </c>
       <c r="T122" t="s">
         <v>20</v>
@@ -8035,7 +8035,7 @@
         <v>3</v>
       </c>
       <c r="S123" t="n">
-        <v>80</v>
+        <v>4.38202663467388</v>
       </c>
       <c r="T123" t="s">
         <v>22</v>
@@ -8097,7 +8097,7 @@
         <v>3</v>
       </c>
       <c r="S124" t="n">
-        <v>600</v>
+        <v>6.39692965521615</v>
       </c>
       <c r="T124" t="s">
         <v>20</v>
@@ -8159,7 +8159,7 @@
         <v>15</v>
       </c>
       <c r="S125" t="n">
-        <v>200</v>
+        <v>5.29831736654804</v>
       </c>
       <c r="T125" t="s">
         <v>22</v>
@@ -8221,7 +8221,7 @@
         <v>5</v>
       </c>
       <c r="S126" t="n">
-        <v>657</v>
+        <v>6.48768401848461</v>
       </c>
       <c r="T126" t="s">
         <v>20</v>
@@ -8283,7 +8283,7 @@
         <v>2</v>
       </c>
       <c r="S127" t="n">
-        <v>75</v>
+        <v>4.31748811353631</v>
       </c>
       <c r="T127" t="s">
         <v>20</v>
@@ -8345,7 +8345,7 @@
         <v>8</v>
       </c>
       <c r="S128" t="n">
-        <v>2412.5</v>
+        <v>7.78841883321314</v>
       </c>
       <c r="T128" t="s">
         <v>22</v>
@@ -8407,7 +8407,7 @@
         <v>14</v>
       </c>
       <c r="S129" t="n">
-        <v>250</v>
+        <v>5.52146091786225</v>
       </c>
       <c r="T129" t="s">
         <v>22</v>
@@ -8469,7 +8469,7 @@
         <v>13</v>
       </c>
       <c r="S130" t="n">
-        <v>155</v>
+        <v>5.04342511691925</v>
       </c>
       <c r="T130" t="s">
         <v>20</v>
@@ -8531,7 +8531,7 @@
         <v>25</v>
       </c>
       <c r="S131" t="n">
-        <v>640</v>
+        <v>6.46146817635372</v>
       </c>
       <c r="T131" t="s">
         <v>20</v>
@@ -8593,7 +8593,7 @@
         <v>5</v>
       </c>
       <c r="S132" t="n">
-        <v>300</v>
+        <v>5.7037824746562</v>
       </c>
       <c r="T132" t="s">
         <v>22</v>
@@ -8655,7 +8655,7 @@
         <v>3</v>
       </c>
       <c r="S133" t="n">
-        <v>110</v>
+        <v>4.70048036579242</v>
       </c>
       <c r="T133" t="s">
         <v>22</v>
@@ -8717,7 +8717,7 @@
         <v>4</v>
       </c>
       <c r="S134" t="n">
-        <v>825</v>
+        <v>6.71538338633468</v>
       </c>
       <c r="T134" t="s">
         <v>20</v>
@@ -8779,7 +8779,7 @@
         <v>16</v>
       </c>
       <c r="S135" t="n">
-        <v>195</v>
+        <v>5.27299955856375</v>
       </c>
       <c r="T135" t="s">
         <v>20</v>
@@ -8841,7 +8841,7 @@
         <v>0</v>
       </c>
       <c r="S136" t="n">
-        <v>450</v>
+        <v>6.10924758276437</v>
       </c>
       <c r="T136" t="s">
         <v>20</v>
@@ -8903,7 +8903,7 @@
         <v>5</v>
       </c>
       <c r="S137" t="n">
-        <v>630</v>
+        <v>6.44571981938558</v>
       </c>
       <c r="T137" t="s">
         <v>20</v>
@@ -8965,7 +8965,7 @@
         <v>3</v>
       </c>
       <c r="S138" t="n">
-        <v>86.5</v>
+        <v>4.46014441393783</v>
       </c>
       <c r="T138" t="s">
         <v>20</v>
@@ -9027,7 +9027,7 @@
         <v>2</v>
       </c>
       <c r="S139" t="n">
-        <v>1300</v>
+        <v>7.17011954344963</v>
       </c>
       <c r="T139" t="s">
         <v>22</v>
@@ -9089,7 +9089,7 @@
         <v>3</v>
       </c>
       <c r="S140" t="n">
-        <v>1000</v>
+        <v>6.90775527898214</v>
       </c>
       <c r="T140" t="s">
         <v>20</v>
@@ -9151,7 +9151,7 @@
         <v>5</v>
       </c>
       <c r="S141" t="n">
-        <v>1800</v>
+        <v>7.49554194388426</v>
       </c>
       <c r="T141" t="s">
         <v>20</v>
@@ -9213,7 +9213,7 @@
         <v>10</v>
       </c>
       <c r="S142" t="n">
-        <v>1310</v>
+        <v>7.1777824161952</v>
       </c>
       <c r="T142" t="s">
         <v>22</v>
@@ -9275,7 +9275,7 @@
         <v>7</v>
       </c>
       <c r="S143" t="n">
-        <v>737.5</v>
+        <v>6.60326608821398</v>
       </c>
       <c r="T143" t="s">
         <v>20</v>
@@ -9337,7 +9337,7 @@
         <v>8</v>
       </c>
       <c r="S144" t="n">
-        <v>625</v>
+        <v>6.4377516497364</v>
       </c>
       <c r="T144" t="s">
         <v>20</v>
@@ -9399,7 +9399,7 @@
         <v>8</v>
       </c>
       <c r="S145" t="n">
-        <v>125</v>
+        <v>4.8283137373023</v>
       </c>
       <c r="T145" t="s">
         <v>20</v>
@@ -9461,7 +9461,7 @@
         <v>4</v>
       </c>
       <c r="S146" t="n">
-        <v>1043.333</v>
+        <v>6.95017567537722</v>
       </c>
       <c r="T146" t="s">
         <v>20</v>
@@ -9523,7 +9523,7 @@
         <v>8</v>
       </c>
       <c r="S147" t="n">
-        <v>725</v>
+        <v>6.58617165485467</v>
       </c>
       <c r="T147" t="s">
         <v>20</v>
@@ -9585,7 +9585,7 @@
         <v>0</v>
       </c>
       <c r="S148" t="n">
-        <v>300</v>
+        <v>5.7037824746562</v>
       </c>
       <c r="T148" t="s">
         <v>22</v>
@@ -9647,7 +9647,7 @@
         <v>6</v>
       </c>
       <c r="S149" t="n">
-        <v>365</v>
+        <v>5.89989735358249</v>
       </c>
       <c r="T149" t="s">
         <v>22</v>
@@ -9709,7 +9709,7 @@
         <v>16</v>
       </c>
       <c r="S150" t="n">
-        <v>75</v>
+        <v>4.31748811353631</v>
       </c>
       <c r="T150" t="s">
         <v>20</v>
@@ -9771,7 +9771,7 @@
         <v>7</v>
       </c>
       <c r="S151" t="n">
-        <v>1183.333</v>
+        <v>7.07609031211117</v>
       </c>
       <c r="T151" t="s">
         <v>20</v>
@@ -9833,7 +9833,7 @@
         <v>3</v>
       </c>
       <c r="S152" t="n">
-        <v>202.5</v>
+        <v>5.31073988654659</v>
       </c>
       <c r="T152" t="s">
         <v>20</v>
@@ -9895,7 +9895,7 @@
         <v>2</v>
       </c>
       <c r="S153" t="n">
-        <v>225</v>
+        <v>5.41610040220442</v>
       </c>
       <c r="T153" t="s">
         <v>22</v>
@@ -9957,7 +9957,7 @@
         <v>2</v>
       </c>
       <c r="S154" t="n">
-        <v>525</v>
+        <v>6.26339826259162</v>
       </c>
       <c r="T154" t="s">
         <v>22</v>
@@ -10019,7 +10019,7 @@
         <v>5</v>
       </c>
       <c r="S155" t="n">
-        <v>265</v>
+        <v>5.57972982598622</v>
       </c>
       <c r="T155" t="s">
         <v>20</v>
@@ -10081,7 +10081,7 @@
         <v>6</v>
       </c>
       <c r="S156" t="n">
-        <v>787.5</v>
+        <v>6.66886337069979</v>
       </c>
       <c r="T156" t="s">
         <v>22</v>
@@ -10143,7 +10143,7 @@
         <v>6</v>
       </c>
       <c r="S157" t="n">
-        <v>800</v>
+        <v>6.68461172766793</v>
       </c>
       <c r="T157" t="s">
         <v>20</v>
@@ -10205,7 +10205,7 @@
         <v>0</v>
       </c>
       <c r="S158" t="n">
-        <v>587.5</v>
+        <v>6.37587624601831</v>
       </c>
       <c r="T158" t="s">
         <v>22</v>
@@ -10267,7 +10267,7 @@
         <v>0</v>
       </c>
       <c r="S159" t="n">
-        <v>145</v>
+        <v>4.97673374242057</v>
       </c>
       <c r="T159" t="s">
         <v>22</v>
@@ -10329,7 +10329,7 @@
         <v>11</v>
       </c>
       <c r="S160" t="n">
-        <v>420</v>
+        <v>6.04025471127741</v>
       </c>
       <c r="T160" t="s">
         <v>22</v>
@@ -10391,7 +10391,7 @@
         <v>1</v>
       </c>
       <c r="S161" t="n">
-        <v>75</v>
+        <v>4.31748811353631</v>
       </c>
       <c r="T161" t="s">
         <v>20</v>
@@ -10453,7 +10453,7 @@
         <v>14</v>
       </c>
       <c r="S162" t="n">
-        <v>575</v>
+        <v>6.35437004079735</v>
       </c>
       <c r="T162" t="s">
         <v>22</v>
@@ -10515,7 +10515,7 @@
         <v>9</v>
       </c>
       <c r="S163" t="n">
-        <v>780</v>
+        <v>6.65929391968364</v>
       </c>
       <c r="T163" t="s">
         <v>22</v>
@@ -10577,7 +10577,7 @@
         <v>3</v>
       </c>
       <c r="S164" t="n">
-        <v>90</v>
+        <v>4.49980967033027</v>
       </c>
       <c r="T164" t="s">
         <v>20</v>
@@ -10639,7 +10639,7 @@
         <v>25</v>
       </c>
       <c r="S165" t="n">
-        <v>150</v>
+        <v>5.01063529409626</v>
       </c>
       <c r="T165" t="s">
         <v>20</v>
@@ -10701,7 +10701,7 @@
         <v>0</v>
       </c>
       <c r="S166" t="n">
-        <v>700</v>
+        <v>6.5510803350434</v>
       </c>
       <c r="T166" t="s">
         <v>20</v>
@@ -10763,7 +10763,7 @@
         <v>7</v>
       </c>
       <c r="S167" t="n">
-        <v>550</v>
+        <v>6.30991827822652</v>
       </c>
       <c r="T167" t="s">
         <v>22</v>
@@ -10825,7 +10825,7 @@
         <v>10</v>
       </c>
       <c r="S168" t="n">
-        <v>650</v>
+        <v>6.47697236288968</v>
       </c>
       <c r="T168" t="s">
         <v>22</v>
@@ -10887,7 +10887,7 @@
         <v>3</v>
       </c>
       <c r="S169" t="n">
-        <v>68</v>
+        <v>4.21950770517611</v>
       </c>
       <c r="T169" t="s">
         <v>22</v>
@@ -10949,7 +10949,7 @@
         <v>6</v>
       </c>
       <c r="S170" t="n">
-        <v>100</v>
+        <v>4.60517018598809</v>
       </c>
       <c r="T170" t="s">
         <v>20</v>
@@ -11011,7 +11011,7 @@
         <v>6</v>
       </c>
       <c r="S171" t="n">
-        <v>670</v>
+        <v>6.50727771238501</v>
       </c>
       <c r="T171" t="s">
         <v>20</v>
@@ -11073,7 +11073,7 @@
         <v>19</v>
       </c>
       <c r="S172" t="n">
-        <v>175</v>
+        <v>5.16478597392351</v>
       </c>
       <c r="T172" t="s">
         <v>22</v>
@@ -11135,7 +11135,7 @@
         <v>8</v>
       </c>
       <c r="S173" t="n">
-        <v>137</v>
+        <v>4.91998092582813</v>
       </c>
       <c r="T173" t="s">
         <v>22</v>
@@ -11197,7 +11197,7 @@
         <v>6</v>
       </c>
       <c r="S174" t="n">
-        <v>2127.333</v>
+        <v>7.66262436147937</v>
       </c>
       <c r="T174" t="s">
         <v>20</v>
@@ -11259,7 +11259,7 @@
         <v>15</v>
       </c>
       <c r="S175" t="n">
-        <v>875</v>
+        <v>6.77422388635761</v>
       </c>
       <c r="T175" t="s">
         <v>20</v>
@@ -11321,7 +11321,7 @@
         <v>8</v>
       </c>
       <c r="S176" t="n">
-        <v>120</v>
+        <v>4.78749174278205</v>
       </c>
       <c r="T176" t="s">
         <v>22</v>
@@ -11383,7 +11383,7 @@
         <v>2</v>
       </c>
       <c r="S177" t="n">
-        <v>140</v>
+        <v>4.9416424226093</v>
       </c>
       <c r="T177" t="s">
         <v>20</v>
@@ -11445,7 +11445,7 @@
         <v>8</v>
       </c>
       <c r="S178" t="n">
-        <v>210</v>
+        <v>5.34710753071747</v>
       </c>
       <c r="T178" t="s">
         <v>20</v>
@@ -11507,7 +11507,7 @@
         <v>5</v>
       </c>
       <c r="S179" t="n">
-        <v>800</v>
+        <v>6.68461172766793</v>
       </c>
       <c r="T179" t="s">
         <v>20</v>
@@ -11569,7 +11569,7 @@
         <v>3</v>
       </c>
       <c r="S180" t="n">
-        <v>240</v>
+        <v>5.48063892334199</v>
       </c>
       <c r="T180" t="s">
         <v>20</v>
@@ -11631,7 +11631,7 @@
         <v>6</v>
       </c>
       <c r="S181" t="n">
-        <v>350</v>
+        <v>5.85793315448346</v>
       </c>
       <c r="T181" t="s">
         <v>22</v>
@@ -11693,7 +11693,7 @@
         <v>22</v>
       </c>
       <c r="S182" t="n">
-        <v>175</v>
+        <v>5.16478597392351</v>
       </c>
       <c r="T182" t="s">
         <v>22</v>
@@ -11755,7 +11755,7 @@
         <v>3</v>
       </c>
       <c r="S183" t="n">
-        <v>200</v>
+        <v>5.29831736654804</v>
       </c>
       <c r="T183" t="s">
         <v>22</v>
@@ -11817,7 +11817,7 @@
         <v>15</v>
       </c>
       <c r="S184" t="n">
-        <v>1940</v>
+        <v>7.57044325205737</v>
       </c>
       <c r="T184" t="s">
         <v>20</v>
@@ -11879,7 +11879,7 @@
         <v>13</v>
       </c>
       <c r="S185" t="n">
-        <v>700</v>
+        <v>6.5510803350434</v>
       </c>
       <c r="T185" t="s">
         <v>20</v>
@@ -11941,7 +11941,7 @@
         <v>1</v>
       </c>
       <c r="S186" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T186" t="s">
         <v>22</v>
@@ -12003,7 +12003,7 @@
         <v>23</v>
       </c>
       <c r="S187" t="n">
-        <v>450</v>
+        <v>6.10924758276437</v>
       </c>
       <c r="T187" t="s">
         <v>20</v>
@@ -12065,7 +12065,7 @@
         <v>14</v>
       </c>
       <c r="S188" t="n">
-        <v>172</v>
+        <v>5.14749447681345</v>
       </c>
       <c r="T188" t="s">
         <v>22</v>
@@ -12127,7 +12127,7 @@
         <v>15</v>
       </c>
       <c r="S189" t="n">
-        <v>1260</v>
+        <v>7.13886699994552</v>
       </c>
       <c r="T189" t="s">
         <v>22</v>
@@ -12189,7 +12189,7 @@
         <v>6</v>
       </c>
       <c r="S190" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T190" t="s">
         <v>20</v>
@@ -12251,7 +12251,7 @@
         <v>4</v>
       </c>
       <c r="S191" t="n">
-        <v>190</v>
+        <v>5.24702407216049</v>
       </c>
       <c r="T191" t="s">
         <v>22</v>
@@ -12313,7 +12313,7 @@
         <v>9</v>
       </c>
       <c r="S192" t="n">
-        <v>580</v>
+        <v>6.36302810354046</v>
       </c>
       <c r="T192" t="s">
         <v>22</v>
@@ -12375,7 +12375,7 @@
         <v>12</v>
       </c>
       <c r="S193" t="n">
-        <v>130</v>
+        <v>4.86753445045558</v>
       </c>
       <c r="T193" t="s">
         <v>20</v>
@@ -12437,7 +12437,7 @@
         <v>3</v>
       </c>
       <c r="S194" t="n">
-        <v>450</v>
+        <v>6.10924758276437</v>
       </c>
       <c r="T194" t="s">
         <v>22</v>
@@ -12499,7 +12499,7 @@
         <v>4</v>
       </c>
       <c r="S195" t="n">
-        <v>300</v>
+        <v>5.7037824746562</v>
       </c>
       <c r="T195" t="s">
         <v>22</v>
@@ -12561,7 +12561,7 @@
         <v>4</v>
       </c>
       <c r="S196" t="n">
-        <v>250</v>
+        <v>5.52146091786225</v>
       </c>
       <c r="T196" t="s">
         <v>22</v>
@@ -12623,7 +12623,7 @@
         <v>8</v>
       </c>
       <c r="S197" t="n">
-        <v>1050</v>
+        <v>6.95654544315157</v>
       </c>
       <c r="T197" t="s">
         <v>22</v>
@@ -12685,7 +12685,7 @@
         <v>8</v>
       </c>
       <c r="S198" t="n">
-        <v>215</v>
+        <v>5.37063802812766</v>
       </c>
       <c r="T198" t="s">
         <v>22</v>
@@ -12747,7 +12747,7 @@
         <v>7</v>
       </c>
       <c r="S199" t="n">
-        <v>400</v>
+        <v>5.99146454710798</v>
       </c>
       <c r="T199" t="s">
         <v>22</v>
@@ -12809,7 +12809,7 @@
         <v>4</v>
       </c>
       <c r="S200" t="n">
-        <v>560</v>
+        <v>6.32793678372919</v>
       </c>
       <c r="T200" t="s">
         <v>22</v>
@@ -12871,7 +12871,7 @@
         <v>6</v>
       </c>
       <c r="S201" t="n">
-        <v>1670</v>
+        <v>7.4205789054108</v>
       </c>
       <c r="T201" t="s">
         <v>22</v>
@@ -12933,7 +12933,7 @@
         <v>0</v>
       </c>
       <c r="S202" t="n">
-        <v>487.5</v>
+        <v>6.1892902904379</v>
       </c>
       <c r="T202" t="s">
         <v>22</v>
@@ -12995,7 +12995,7 @@
         <v>0</v>
       </c>
       <c r="S203" t="n">
-        <v>425</v>
+        <v>6.05208916892442</v>
       </c>
       <c r="T203" t="s">
         <v>22</v>
@@ -13057,7 +13057,7 @@
         <v>16</v>
       </c>
       <c r="S204" t="n">
-        <v>500</v>
+        <v>6.21460809842219</v>
       </c>
       <c r="T204" t="s">
         <v>22</v>
@@ -13119,7 +13119,7 @@
         <v>1</v>
       </c>
       <c r="S205" t="n">
-        <v>250</v>
+        <v>5.52146091786225</v>
       </c>
       <c r="T205" t="s">
         <v>22</v>
@@ -13181,7 +13181,7 @@
         <v>2</v>
       </c>
       <c r="S206" t="n">
-        <v>400</v>
+        <v>5.99146454710798</v>
       </c>
       <c r="T206" t="s">
         <v>22</v>
@@ -13243,7 +13243,7 @@
         <v>6</v>
       </c>
       <c r="S207" t="n">
-        <v>450</v>
+        <v>6.10924758276437</v>
       </c>
       <c r="T207" t="s">
         <v>22</v>
@@ -13305,7 +13305,7 @@
         <v>19</v>
       </c>
       <c r="S208" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T208" t="s">
         <v>20</v>
@@ -13367,7 +13367,7 @@
         <v>15</v>
       </c>
       <c r="S209" t="n">
-        <v>70</v>
+        <v>4.24849524204936</v>
       </c>
       <c r="T209" t="s">
         <v>22</v>
@@ -13429,7 +13429,7 @@
         <v>29</v>
       </c>
       <c r="S210" t="n">
-        <v>875</v>
+        <v>6.77422388635761</v>
       </c>
       <c r="T210" t="s">
         <v>20</v>
@@ -13491,7 +13491,7 @@
         <v>9</v>
       </c>
       <c r="S211" t="n">
-        <v>190</v>
+        <v>5.24702407216049</v>
       </c>
       <c r="T211" t="s">
         <v>20</v>
@@ -13553,7 +13553,7 @@
         <v>2</v>
       </c>
       <c r="S212" t="n">
-        <v>191</v>
+        <v>5.25227342804663</v>
       </c>
       <c r="T212" t="s">
         <v>20</v>
@@ -13615,7 +13615,7 @@
         <v>5</v>
       </c>
       <c r="S213" t="n">
-        <v>740</v>
+        <v>6.60665018619822</v>
       </c>
       <c r="T213" t="s">
         <v>20</v>
@@ -13677,7 +13677,7 @@
         <v>16</v>
       </c>
       <c r="S214" t="n">
-        <v>250</v>
+        <v>5.52146091786225</v>
       </c>
       <c r="T214" t="s">
         <v>20</v>
@@ -13739,7 +13739,7 @@
         <v>13</v>
       </c>
       <c r="S215" t="n">
-        <v>140</v>
+        <v>4.9416424226093</v>
       </c>
       <c r="T215" t="s">
         <v>20</v>
@@ -13801,7 +13801,7 @@
         <v>6</v>
       </c>
       <c r="S216" t="n">
-        <v>97.5</v>
+        <v>4.5798523780038</v>
       </c>
       <c r="T216" t="s">
         <v>22</v>
@@ -13863,7 +13863,7 @@
         <v>0</v>
       </c>
       <c r="S217" t="n">
-        <v>740</v>
+        <v>6.60665018619822</v>
       </c>
       <c r="T217" t="s">
         <v>22</v>
@@ -13925,7 +13925,7 @@
         <v>17</v>
       </c>
       <c r="S218" t="n">
-        <v>140</v>
+        <v>4.9416424226093</v>
       </c>
       <c r="T218" t="s">
         <v>20</v>
@@ -13987,7 +13987,7 @@
         <v>7</v>
       </c>
       <c r="S219" t="n">
-        <v>341.667</v>
+        <v>5.83383657851368</v>
       </c>
       <c r="T219" t="s">
         <v>22</v>
@@ -14049,7 +14049,7 @@
         <v>1</v>
       </c>
       <c r="S220" t="n">
-        <v>1000</v>
+        <v>6.90775527898214</v>
       </c>
       <c r="T220" t="s">
         <v>22</v>
@@ -14111,7 +14111,7 @@
         <v>18</v>
       </c>
       <c r="S221" t="n">
-        <v>100</v>
+        <v>4.60517018598809</v>
       </c>
       <c r="T221" t="s">
         <v>22</v>
@@ -14173,7 +14173,7 @@
         <v>3</v>
       </c>
       <c r="S222" t="n">
-        <v>90</v>
+        <v>4.49980967033027</v>
       </c>
       <c r="T222" t="s">
         <v>22</v>
@@ -14235,7 +14235,7 @@
         <v>17</v>
       </c>
       <c r="S223" t="n">
-        <v>200</v>
+        <v>5.29831736654804</v>
       </c>
       <c r="T223" t="s">
         <v>20</v>
@@ -14297,7 +14297,7 @@
         <v>11</v>
       </c>
       <c r="S224" t="n">
-        <v>135</v>
+        <v>4.90527477843843</v>
       </c>
       <c r="T224" t="s">
         <v>22</v>
@@ -14359,7 +14359,7 @@
         <v>32</v>
       </c>
       <c r="S225" t="n">
-        <v>155</v>
+        <v>5.04342511691925</v>
       </c>
       <c r="T225" t="s">
         <v>20</v>
@@ -14421,7 +14421,7 @@
         <v>15</v>
       </c>
       <c r="S226" t="n">
-        <v>475</v>
+        <v>6.16331480403464</v>
       </c>
       <c r="T226" t="s">
         <v>22</v>
@@ -14483,7 +14483,7 @@
         <v>7</v>
       </c>
       <c r="S227" t="n">
-        <v>1450</v>
+        <v>7.27931883541462</v>
       </c>
       <c r="T227" t="s">
         <v>20</v>
@@ -14545,7 +14545,7 @@
         <v>22</v>
       </c>
       <c r="S228" t="n">
-        <v>150</v>
+        <v>5.01063529409626</v>
       </c>
       <c r="T228" t="s">
         <v>20</v>
@@ -14607,7 +14607,7 @@
         <v>6</v>
       </c>
       <c r="S229" t="n">
-        <v>105</v>
+        <v>4.65396035015752</v>
       </c>
       <c r="T229" t="s">
         <v>22</v>
@@ -14669,7 +14669,7 @@
         <v>17</v>
       </c>
       <c r="S230" t="n">
-        <v>350</v>
+        <v>5.85793315448346</v>
       </c>
       <c r="T230" t="s">
         <v>22</v>
@@ -14731,7 +14731,7 @@
         <v>16</v>
       </c>
       <c r="S231" t="n">
-        <v>90</v>
+        <v>4.49980967033027</v>
       </c>
       <c r="T231" t="s">
         <v>20</v>
@@ -14793,7 +14793,7 @@
         <v>17</v>
       </c>
       <c r="S232" t="n">
-        <v>530</v>
+        <v>6.27287700654617</v>
       </c>
       <c r="T232" t="s">
         <v>22</v>
@@ -14855,7 +14855,7 @@
         <v>7</v>
       </c>
       <c r="S233" t="n">
-        <v>341.667</v>
+        <v>5.83383657851368</v>
       </c>
       <c r="T233" t="s">
         <v>22</v>
@@ -14917,7 +14917,7 @@
         <v>6</v>
       </c>
       <c r="S234" t="n">
-        <v>940</v>
+        <v>6.84587987526405</v>
       </c>
       <c r="T234" t="s">
         <v>22</v>
@@ -14979,7 +14979,7 @@
         <v>13</v>
       </c>
       <c r="S235" t="n">
-        <v>350</v>
+        <v>5.85793315448346</v>
       </c>
       <c r="T235" t="s">
         <v>22</v>
@@ -15041,7 +15041,7 @@
         <v>3</v>
       </c>
       <c r="S236" t="n">
-        <v>326.667</v>
+        <v>5.78894130340415</v>
       </c>
       <c r="T236" t="s">
         <v>20</v>
@@ -15103,7 +15103,7 @@
         <v>4</v>
       </c>
       <c r="S237" t="n">
-        <v>250</v>
+        <v>5.52146091786225</v>
       </c>
       <c r="T237" t="s">
         <v>20</v>
@@ -15165,7 +15165,7 @@
         <v>4</v>
       </c>
       <c r="S238" t="n">
-        <v>740</v>
+        <v>6.60665018619822</v>
       </c>
       <c r="T238" t="s">
         <v>20</v>
@@ -15227,7 +15227,7 @@
         <v>3</v>
       </c>
       <c r="S239" t="n">
-        <v>425</v>
+        <v>6.05208916892442</v>
       </c>
       <c r="T239" t="s">
         <v>22</v>
@@ -15289,7 +15289,7 @@
         <v>9</v>
       </c>
       <c r="S240" t="n">
-        <v>925</v>
+        <v>6.82979373751242</v>
       </c>
       <c r="T240" t="s">
         <v>20</v>
@@ -15351,7 +15351,7 @@
         <v>11</v>
       </c>
       <c r="S241" t="n">
-        <v>185</v>
+        <v>5.22035582507832</v>
       </c>
       <c r="T241" t="s">
         <v>22</v>
@@ -15413,7 +15413,7 @@
         <v>8</v>
       </c>
       <c r="S242" t="n">
-        <v>920</v>
+        <v>6.82437367004309</v>
       </c>
       <c r="T242" t="s">
         <v>22</v>
@@ -15475,7 +15475,7 @@
         <v>1</v>
       </c>
       <c r="S243" t="n">
-        <v>286.667</v>
+        <v>5.65832126336946</v>
       </c>
       <c r="T243" t="s">
         <v>20</v>
@@ -15537,7 +15537,7 @@
         <v>5</v>
       </c>
       <c r="S244" t="n">
-        <v>245</v>
+        <v>5.50125821054473</v>
       </c>
       <c r="T244" t="s">
         <v>22</v>
@@ -15599,7 +15599,7 @@
         <v>4</v>
       </c>
       <c r="S245" t="n">
-        <v>235</v>
+        <v>5.45958551414416</v>
       </c>
       <c r="T245" t="s">
         <v>22</v>
@@ -15661,7 +15661,7 @@
         <v>18</v>
       </c>
       <c r="S246" t="n">
-        <v>1150</v>
+        <v>7.0475172213573</v>
       </c>
       <c r="T246" t="s">
         <v>20</v>
@@ -15723,7 +15723,7 @@
         <v>20</v>
       </c>
       <c r="S247" t="n">
-        <v>160</v>
+        <v>5.07517381523383</v>
       </c>
       <c r="T247" t="s">
         <v>20</v>
@@ -15785,7 +15785,7 @@
         <v>11</v>
       </c>
       <c r="S248" t="n">
-        <v>425</v>
+        <v>6.05208916892442</v>
       </c>
       <c r="T248" t="s">
         <v>22</v>
@@ -15847,7 +15847,7 @@
         <v>0</v>
       </c>
       <c r="S249" t="n">
-        <v>900</v>
+        <v>6.80239476332431</v>
       </c>
       <c r="T249" t="s">
         <v>20</v>
@@ -15909,7 +15909,7 @@
         <v>6</v>
       </c>
       <c r="S250" t="n">
-        <v>500</v>
+        <v>6.21460809842219</v>
       </c>
       <c r="T250" t="s">
         <v>20</v>
@@ -15971,7 +15971,7 @@
         <v>9</v>
       </c>
       <c r="S251" t="n">
-        <v>277.5</v>
+        <v>5.62582093318649</v>
       </c>
       <c r="T251" t="s">
         <v>20</v>
@@ -16033,7 +16033,7 @@
         <v>16</v>
       </c>
       <c r="S252" t="n">
-        <v>750</v>
+        <v>6.62007320653036</v>
       </c>
       <c r="T252" t="s">
         <v>20</v>
@@ -16095,7 +16095,7 @@
         <v>9</v>
       </c>
       <c r="S253" t="n">
-        <v>160</v>
+        <v>5.07517381523383</v>
       </c>
       <c r="T253" t="s">
         <v>20</v>
@@ -16157,7 +16157,7 @@
         <v>13</v>
       </c>
       <c r="S254" t="n">
-        <v>1300</v>
+        <v>7.17011954344963</v>
       </c>
       <c r="T254" t="s">
         <v>20</v>
@@ -16219,7 +16219,7 @@
         <v>3</v>
       </c>
       <c r="S255" t="n">
-        <v>525</v>
+        <v>6.26339826259162</v>
       </c>
       <c r="T255" t="s">
         <v>20</v>
@@ -16281,7 +16281,7 @@
         <v>17</v>
       </c>
       <c r="S256" t="n">
-        <v>550</v>
+        <v>6.30991827822652</v>
       </c>
       <c r="T256" t="s">
         <v>20</v>
@@ -16343,7 +16343,7 @@
         <v>19</v>
       </c>
       <c r="S257" t="n">
-        <v>1600</v>
+        <v>7.37775890822787</v>
       </c>
       <c r="T257" t="s">
         <v>22</v>
@@ -16405,7 +16405,7 @@
         <v>11</v>
       </c>
       <c r="S258" t="n">
-        <v>120</v>
+        <v>4.78749174278205</v>
       </c>
       <c r="T258" t="s">
         <v>20</v>
@@ -16467,7 +16467,7 @@
         <v>15</v>
       </c>
       <c r="S259" t="n">
-        <v>165</v>
+        <v>5.10594547390058</v>
       </c>
       <c r="T259" t="s">
         <v>22</v>
@@ -16529,7 +16529,7 @@
         <v>3</v>
       </c>
       <c r="S260" t="n">
-        <v>700</v>
+        <v>6.5510803350434</v>
       </c>
       <c r="T260" t="s">
         <v>20</v>
@@ -16591,7 +16591,7 @@
         <v>20</v>
       </c>
       <c r="S261" t="n">
-        <v>875</v>
+        <v>6.77422388635761</v>
       </c>
       <c r="T261" t="s">
         <v>22</v>
@@ -16653,7 +16653,7 @@
         <v>7</v>
       </c>
       <c r="S262" t="n">
-        <v>385</v>
+        <v>5.95324333428778</v>
       </c>
       <c r="T262" t="s">
         <v>22</v>
@@ -16715,7 +16715,7 @@
         <v>12</v>
       </c>
       <c r="S263" t="n">
-        <v>960</v>
+        <v>6.86693328446188</v>
       </c>
       <c r="T263" t="s">
         <v>22</v>
@@ -16777,7 +16777,7 @@
         <v>3</v>
       </c>
       <c r="S264" t="n">
-        <v>1000</v>
+        <v>6.90775527898214</v>
       </c>
       <c r="T264" t="s">
         <v>22</v>

</xml_diff>